<commit_message>
Automatische test-sync: 2025-06-20 08:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,8 +679,40 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-20 08:30:14</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -700,7 +732,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -718,7 +750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,6 +780,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 09:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,8 +711,40 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sponsoraanvraag</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Zou uw bedrijf bereid zijn om ons sportevenement te sponsoren?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-20 09:00:10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -732,7 +764,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -750,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,6 +822,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 09:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,8 +743,40 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-20 09:30:14</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -764,7 +796,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -782,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -832,6 +864,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 10:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,8 +775,40 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-20 10:00:12</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -796,7 +828,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -837,17 +869,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -857,7 +889,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 10:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,8 +807,40 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-20 10:30:11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -828,7 +860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -869,7 +901,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -879,11 +911,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 11:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,8 +839,40 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-20 11:00:12</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -860,7 +892,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -878,7 +910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -938,6 +970,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 11:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,8 +871,40 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-20 11:30:25</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -892,7 +924,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -910,7 +942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -980,6 +1012,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 12:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,8 +903,40 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-20 12:00:14</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -924,7 +956,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -965,17 +997,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 12:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,8 +935,40 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-20 12:30:28</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -956,7 +988,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1001,7 +1033,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 13:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -967,8 +967,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-20 13:00:12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -988,7 +1020,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1049,17 +1081,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1069,7 +1101,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 13:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,8 +999,48 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw vraag. Onze openingstijden zijn maandag t/m vrijdag van 09:00 tot 17:00 uur. Voor verdere informatie kunt u onze website raadplegen of telefonisch contact met ons opnemen.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-20 13:30:12</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1020,7 +1060,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1038,7 +1078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1118,6 +1158,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 14:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1039,8 +1039,40 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-20 14:00:11</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1060,7 +1092,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1115,7 +1147,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 14:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,8 +1071,40 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-20 14:30:44</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1092,7 +1124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1133,7 +1165,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1143,11 +1175,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 15:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,8 +1103,40 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-20 15:00:10</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1124,7 +1156,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1189,7 +1221,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 15:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,8 +1135,48 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Beste [naam],
+Bedankt voor je interesse. Wij zijn geopend van maandag tot en met vrijdag van 9:00 tot 18:00 uur en op zaterdag van 10:00 tot 15:00 uur. Op zondag zijn wij gesloten. Mocht je nog verdere vragen hebben, laat het ons gerust weten.
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-20 15:30:13</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1156,7 +1196,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1227,17 +1267,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1247,7 +1287,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1257,7 +1297,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 16:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,8 +1175,40 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-20 16:00:16</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1196,7 +1228,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1267,7 +1299,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1277,11 +1309,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-20 16:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-20.xlsx
+++ b/logs/mail_log_2025-06-20.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1207,8 +1207,40 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-20 16:30:39</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1228,7 +1260,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1246,7 +1278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1336,6 +1368,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>